<commit_message>
Update Tournament Era Worksheet.xlsx
</commit_message>
<xml_diff>
--- a/Tournament Era Worksheet.xlsx
+++ b/Tournament Era Worksheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OOTP Analytics\Tournament Era\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\OOTPResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483A2FBE-92C9-4221-912F-C1968C634EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135237BD-D401-437F-932B-8F116DDFC598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{06CCA8F3-D635-4773-A702-800788336C23}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{06CCA8F3-D635-4773-A702-800788336C23}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="4" r:id="rId1"/>
@@ -653,7 +653,6 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -691,6 +690,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1035,7 +1035,7 @@
   <dimension ref="B1:AA38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,429 +1049,429 @@
   <sheetData>
     <row r="1" spans="2:27" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="P2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="S2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="T2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="U2" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="V2" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="X2" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="Y2" s="13" t="s">
+      <c r="Y2" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="Z2" s="13" t="s">
+      <c r="Z2" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="AA2" s="14" t="s">
+      <c r="AA2" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="15">
         <f>Batting!$D$14</f>
         <v>185553</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <f>Batting!$G$14</f>
         <v>42554</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="15">
         <f>Batting!$H$14</f>
         <v>28589</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="15">
         <f>Batting!$I$14</f>
         <v>8486</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="15">
         <f>Batting!$J$14</f>
         <v>866</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <f>Batting!$K$14</f>
         <v>4613</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="15">
         <f>Batting!$AL$14</f>
         <v>14562</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="15">
         <f>Batting!$W$14</f>
         <v>1549</v>
       </c>
-      <c r="K3" s="16">
+      <c r="K3" s="15">
         <f>Batting!$P$14</f>
         <v>34306</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="15">
         <f>Batting!$M$14</f>
         <v>2959</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="15">
         <f>Batting!$N$14</f>
         <v>1129</v>
       </c>
-      <c r="N3" s="16">
+      <c r="N3" s="15">
         <f>Batting!$Q$14</f>
         <v>0.25700000000000001</v>
       </c>
-      <c r="O3" s="16">
+      <c r="O3" s="15">
         <f>Batting!$R$14</f>
         <v>0.32500000000000001</v>
       </c>
-      <c r="P3" s="16">
+      <c r="P3" s="15">
         <f>Batting!$S$14</f>
         <v>0.40300000000000002</v>
       </c>
-      <c r="Q3" s="17">
+      <c r="Q3" s="16">
         <f>Batting!$AK$14</f>
         <v>0.25647074728766012</v>
       </c>
-      <c r="R3" s="18">
+      <c r="R3" s="17">
         <f>Batting!$AB$14</f>
         <v>8.7559670781893004</v>
       </c>
-      <c r="S3" s="18">
+      <c r="S3" s="17">
         <f>Batting!$AC$14</f>
         <v>5.882510288065844</v>
       </c>
-      <c r="T3" s="18">
+      <c r="T3" s="17">
         <f>Batting!$AD$14</f>
         <v>1.7460905349794238</v>
       </c>
-      <c r="U3" s="18">
+      <c r="U3" s="17">
         <f>Batting!$AE$14</f>
         <v>0.17818930041152264</v>
       </c>
-      <c r="V3" s="18">
+      <c r="V3" s="17">
         <f>Batting!$AF$14</f>
         <v>0.94917695473251029</v>
       </c>
-      <c r="W3" s="18">
+      <c r="W3" s="17">
         <f>Batting!$AG$14</f>
         <v>0.60884773662551439</v>
       </c>
-      <c r="X3" s="18">
+      <c r="X3" s="17">
         <f>Batting!$AH$14</f>
         <v>2.9962962962962965</v>
       </c>
-      <c r="Y3" s="18">
+      <c r="Y3" s="17">
         <f>Batting!$AI$14</f>
         <v>7.0588477366255145</v>
       </c>
-      <c r="Z3" s="18">
+      <c r="Z3" s="17">
         <f>Batting!$AJ$14</f>
         <v>26.282921810699587</v>
       </c>
-      <c r="AA3" s="19">
+      <c r="AA3" s="18">
         <f>Pitching!$AI$14</f>
         <v>0.62345679012345678</v>
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <f>C16</f>
-        <v>1884</v>
-      </c>
-      <c r="C4" s="16">
+        <v>1925</v>
+      </c>
+      <c r="C4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,4,FALSE)</f>
-        <v>114727</v>
-      </c>
-      <c r="D4" s="16">
+        <v>136241</v>
+      </c>
+      <c r="D4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,7,FALSE)</f>
-        <v>26593</v>
-      </c>
-      <c r="E4" s="16">
+        <v>34798</v>
+      </c>
+      <c r="E4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,8,FALSE)</f>
-        <v>20347</v>
-      </c>
-      <c r="F4" s="16">
+        <v>25558</v>
+      </c>
+      <c r="F4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,9,FALSE)</f>
-        <v>4020</v>
-      </c>
-      <c r="G4" s="16">
+        <v>5823</v>
+      </c>
+      <c r="G4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,10,FALSE)</f>
-        <v>1537</v>
-      </c>
-      <c r="H4" s="16">
+        <v>1681</v>
+      </c>
+      <c r="H4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,11,FALSE)</f>
-        <v>689</v>
-      </c>
-      <c r="I4" s="16">
+        <v>1736</v>
+      </c>
+      <c r="I4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,38,FALSE)</f>
-        <v>4947</v>
-      </c>
-      <c r="J4" s="16">
+        <v>10944</v>
+      </c>
+      <c r="J4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,23,FALSE)</f>
-        <v>468</v>
-      </c>
-      <c r="K4" s="16">
+        <v>495</v>
+      </c>
+      <c r="K4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,16,FALSE)</f>
-        <v>4335</v>
-      </c>
-      <c r="L4" s="16">
+        <v>6665</v>
+      </c>
+      <c r="L4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,13,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="16">
+        <v>2370</v>
+      </c>
+      <c r="M4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,14,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="17">
+        <v>1103</v>
+      </c>
+      <c r="N4" s="16">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,17,FALSE)</f>
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="O4" s="17">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="O4" s="16">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,18,FALSE)</f>
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="P4" s="17">
+        <v>0.35</v>
+      </c>
+      <c r="P4" s="16">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,19,FALSE)</f>
-        <v>0.32700000000000001</v>
-      </c>
-      <c r="Q4" s="17">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="Q4" s="16">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,37,FALSE)</f>
-        <v>0.23612845592189821</v>
-      </c>
-      <c r="R4" s="18">
+        <v>0.25862015018773465</v>
+      </c>
+      <c r="R4" s="17">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,28,FALSE)</f>
-        <v>8.6509433962264151</v>
-      </c>
-      <c r="S4" s="18">
+        <v>9.9366076527698457</v>
+      </c>
+      <c r="S4" s="17">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,29,FALSE)</f>
-        <v>6.6190631099544568</v>
-      </c>
-      <c r="T4" s="18">
+        <v>7.2981153626499147</v>
+      </c>
+      <c r="T4" s="17">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,30,FALSE)</f>
-        <v>1.3077423552374756</v>
-      </c>
-      <c r="U4" s="18">
+        <v>1.6627641347801256</v>
+      </c>
+      <c r="U4" s="17">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,31,FALSE)</f>
-        <v>0.5</v>
-      </c>
-      <c r="V4" s="18">
+        <v>0.480011422044546</v>
+      </c>
+      <c r="V4" s="17">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,32,FALSE)</f>
-        <v>0.22413793103448276</v>
-      </c>
-      <c r="W4" s="18">
+        <v>0.49571673329525984</v>
+      </c>
+      <c r="W4" s="17">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,33,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="X4" s="18">
+        <v>0.67675613934894341</v>
+      </c>
+      <c r="X4" s="17">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,34,FALSE)</f>
-        <v>1.6093038386467144</v>
-      </c>
-      <c r="Y4" s="18">
+        <v>3.1250713877784122</v>
+      </c>
+      <c r="Y4" s="17">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,35,FALSE)</f>
-        <v>1.4102147039687702</v>
-      </c>
-      <c r="Z4" s="18">
+        <v>1.9031981724728726</v>
+      </c>
+      <c r="Z4" s="17">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,36,FALSE)</f>
-        <v>33.925829538061159</v>
-      </c>
-      <c r="AA4" s="19">
+        <v>32.098229583095375</v>
+      </c>
+      <c r="AA4" s="18">
         <f>VLOOKUP($B$4,Pitching!$A$1:$AL$153,35,FALSE)</f>
-        <v>4.7348731294729998</v>
+        <v>1.0937188434695913</v>
       </c>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22">
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21">
         <f>N4-N3</f>
-        <v>-1.4000000000000012E-2</v>
-      </c>
-      <c r="O5" s="22">
+        <v>3.0999999999999972E-2</v>
+      </c>
+      <c r="O5" s="21">
         <f t="shared" ref="O5:AA5" si="0">O4-O3</f>
-        <v>-4.5999999999999985E-2</v>
-      </c>
-      <c r="P5" s="22">
+        <v>2.4999999999999967E-2</v>
+      </c>
+      <c r="P5" s="21">
         <f t="shared" si="0"/>
-        <v>-7.6000000000000012E-2</v>
-      </c>
-      <c r="Q5" s="23">
+        <v>3.999999999999948E-3</v>
+      </c>
+      <c r="Q5" s="22">
         <f t="shared" si="0"/>
-        <v>-2.0342291365761905E-2</v>
-      </c>
-      <c r="R5" s="24">
+        <v>2.1494029000745374E-3</v>
+      </c>
+      <c r="R5" s="23">
         <f t="shared" si="0"/>
-        <v>-0.10502368196288536</v>
-      </c>
-      <c r="S5" s="24">
+        <v>1.1806405745805453</v>
+      </c>
+      <c r="S5" s="23">
         <f t="shared" si="0"/>
-        <v>0.73655282188861282</v>
-      </c>
-      <c r="T5" s="24">
+        <v>1.4156050745840707</v>
+      </c>
+      <c r="T5" s="23">
         <f t="shared" si="0"/>
-        <v>-0.43834817974194817</v>
-      </c>
-      <c r="U5" s="24">
+        <v>-8.3326400199298156E-2</v>
+      </c>
+      <c r="U5" s="23">
         <f t="shared" si="0"/>
-        <v>0.32181069958847736</v>
-      </c>
-      <c r="V5" s="24">
+        <v>0.30182212163302335</v>
+      </c>
+      <c r="V5" s="23">
         <f t="shared" si="0"/>
-        <v>-0.72503902369802753</v>
-      </c>
-      <c r="W5" s="24">
+        <v>-0.45346022143725045</v>
+      </c>
+      <c r="W5" s="23">
         <f t="shared" si="0"/>
-        <v>-0.60884773662551439</v>
-      </c>
-      <c r="X5" s="24">
+        <v>6.7908402723429018E-2</v>
+      </c>
+      <c r="X5" s="23">
         <f t="shared" si="0"/>
-        <v>-1.386992457649582</v>
-      </c>
-      <c r="Y5" s="24">
+        <v>0.12877509148211574</v>
+      </c>
+      <c r="Y5" s="23">
         <f t="shared" si="0"/>
-        <v>-5.6486330326567442</v>
-      </c>
-      <c r="Z5" s="24">
+        <v>-5.1556495641526414</v>
+      </c>
+      <c r="Z5" s="23">
         <f t="shared" si="0"/>
-        <v>7.6429077273615711</v>
-      </c>
-      <c r="AA5" s="25">
+        <v>5.8153077723957871</v>
+      </c>
+      <c r="AA5" s="24">
         <f t="shared" si="0"/>
-        <v>4.1114163393495433</v>
+        <v>0.47026205334613447</v>
       </c>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="L6" s="27" t="s">
+      <c r="L6" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="27" t="s">
+      <c r="M6" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="N6" s="27" t="s">
+      <c r="N6" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="27" t="s">
+      <c r="O6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="27" t="s">
+      <c r="P6" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="Q6" s="27" t="s">
+      <c r="Q6" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="R6" s="27" t="s">
+      <c r="R6" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="S6" s="27" t="s">
+      <c r="S6" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="T6" s="28" t="s">
+      <c r="T6" s="27" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>69</v>
       </c>
       <c r="C7" s="7">
@@ -1542,361 +1542,361 @@
         <f>Pitching!AH14</f>
         <v>-7.548471319929817E-2</v>
       </c>
-      <c r="T7" s="30">
+      <c r="T7" s="29">
         <f>Pitching!$E$14</f>
         <v>4.38</v>
       </c>
     </row>
     <row r="8" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B8" s="31">
+      <c r="B8" s="30">
         <f>C16</f>
-        <v>1884</v>
+        <v>1925</v>
       </c>
       <c r="C8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,24,FALSE)</f>
-        <v>115408</v>
+        <v>136187</v>
       </c>
       <c r="D8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,13,FALSE)</f>
-        <v>26945</v>
+        <v>30933</v>
       </c>
       <c r="E8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,15,FALSE)</f>
-        <v>16740</v>
+        <v>18345</v>
       </c>
       <c r="F8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,16,FALSE)</f>
-        <v>9307</v>
+        <v>15658</v>
       </c>
       <c r="G8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,14,FALSE)</f>
-        <v>26592</v>
+        <v>34807</v>
       </c>
       <c r="H8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,17,FALSE)</f>
-        <v>689</v>
+        <v>1169</v>
       </c>
       <c r="I8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,20,FALSE)</f>
-        <v>14837</v>
+        <v>10380</v>
       </c>
       <c r="J8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,36,FALSE)</f>
-        <v>4947</v>
+        <v>10827</v>
       </c>
       <c r="K8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,21,FALSE)</f>
-        <v>472</v>
+        <v>648</v>
       </c>
       <c r="L8" s="9">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,30,FALSE)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M8" s="9">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,37,FALSE)</f>
-        <v>1.6523659305993692</v>
+        <v>3.1501309281350016</v>
       </c>
       <c r="N8" s="9">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,28,FALSE)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="O8" s="9">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,6,FALSE)</f>
-        <v>3.11</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="P8" s="9">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,38,FALSE)</f>
-        <v>5.5913898682501397</v>
+        <v>5.337503636892639</v>
       </c>
       <c r="Q8" s="8">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,25,FALSE)</f>
-        <v>1.17</v>
+        <v>1.4750000000000001</v>
       </c>
       <c r="R8" s="9">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,33,FALSE)</f>
-        <v>3.1034776396362962</v>
+        <v>4.0400488475091327</v>
       </c>
       <c r="S8" s="9">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,34,FALSE)</f>
-        <v>-6.5223603637036831E-3</v>
-      </c>
-      <c r="T8" s="30">
+        <v>-0.51995115249086687</v>
+      </c>
+      <c r="T8" s="29">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,5,FALSE)</f>
-        <v>5.45</v>
+        <v>5.24</v>
       </c>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="34">
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33">
         <f>L8-L7</f>
-        <v>-2.0999999999999996</v>
-      </c>
-      <c r="M9" s="34">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="M9" s="33">
         <f t="shared" ref="M9:T9" si="1">M8-M7</f>
-        <v>-1.3740049552037652</v>
-      </c>
-      <c r="N9" s="34">
+        <v>0.12376004233186721</v>
+      </c>
+      <c r="N9" s="33">
         <f t="shared" si="1"/>
-        <v>-0.8</v>
-      </c>
-      <c r="O9" s="34">
+        <v>-0.7</v>
+      </c>
+      <c r="O9" s="33">
         <f t="shared" si="1"/>
-        <v>-0.96000000000000041</v>
-      </c>
-      <c r="P9" s="34">
+        <v>0.48999999999999932</v>
+      </c>
+      <c r="P9" s="33">
         <f t="shared" si="1"/>
-        <v>1.1630207682162705</v>
-      </c>
-      <c r="Q9" s="34">
+        <v>0.90913453685876977</v>
+      </c>
+      <c r="Q9" s="33">
         <f t="shared" si="1"/>
-        <v>-0.17700000000000005</v>
-      </c>
-      <c r="R9" s="34">
+        <v>0.12800000000000011</v>
+      </c>
+      <c r="R9" s="33">
         <f t="shared" si="1"/>
-        <v>-0.89103764716440592</v>
-      </c>
-      <c r="S9" s="34">
+        <v>4.553356070843062E-2</v>
+      </c>
+      <c r="S9" s="33">
         <f t="shared" si="1"/>
-        <v>6.8962352835594487E-2</v>
-      </c>
-      <c r="T9" s="35">
+        <v>-0.4444664392915687</v>
+      </c>
+      <c r="T9" s="34">
         <f t="shared" si="1"/>
-        <v>1.0700000000000003</v>
+        <v>0.86000000000000032</v>
       </c>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="37" t="s">
+      <c r="I10" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="J10" s="37" t="s">
+      <c r="J10" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="K10" s="37" t="s">
+      <c r="K10" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="L10" s="37" t="s">
+      <c r="L10" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="M10" s="37" t="s">
+      <c r="M10" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="N10" s="37" t="s">
+      <c r="N10" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="O10" s="38" t="s">
+      <c r="O10" s="37" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="39">
         <f>FGGuts!$B$14</f>
         <v>0.32100000000000001</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="39">
         <f>FGGuts!$C$14</f>
         <v>1.2509999999999999</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="39">
         <f>FGGuts!$D$14</f>
         <v>0.70099999999999996</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="39">
         <f>FGGuts!$E$14</f>
         <v>0.73199999999999998</v>
       </c>
-      <c r="G11" s="40">
+      <c r="G11" s="39">
         <f>FGGuts!$F$14</f>
         <v>0.89500000000000002</v>
       </c>
-      <c r="H11" s="40">
+      <c r="H11" s="39">
         <f>FGGuts!$G$14</f>
         <v>1.27</v>
       </c>
-      <c r="I11" s="40">
+      <c r="I11" s="39">
         <f>FGGuts!$H$14</f>
         <v>1.6080000000000001</v>
       </c>
-      <c r="J11" s="40">
+      <c r="J11" s="39">
         <f>FGGuts!$I$14</f>
         <v>2.0720000000000001</v>
       </c>
-      <c r="K11" s="40">
+      <c r="K11" s="39">
         <f>FGGuts!$J$14</f>
         <v>0.2</v>
       </c>
-      <c r="L11" s="40">
+      <c r="L11" s="39">
         <f>FGGuts!$K$14</f>
         <v>-0.40300000000000002</v>
       </c>
-      <c r="M11" s="40">
+      <c r="M11" s="39">
         <f>FGGuts!$L$14</f>
         <v>0.115</v>
       </c>
-      <c r="N11" s="40">
+      <c r="N11" s="39">
         <f>FGGuts!$M$14</f>
         <v>9.6430000000000007</v>
       </c>
-      <c r="O11" s="41">
+      <c r="O11" s="40">
         <f>FGGuts!$N$14</f>
         <v>3.0779999999999998</v>
       </c>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B12" s="42">
+      <c r="B12" s="41">
         <f>C16</f>
-        <v>1884</v>
-      </c>
-      <c r="C12" s="40">
+        <v>1925</v>
+      </c>
+      <c r="C12" s="39">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,2,FALSE)</f>
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="D12" s="40">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="D12" s="39">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,3,FALSE)</f>
-        <v>1.288</v>
-      </c>
-      <c r="E12" s="40">
+        <v>1.1950000000000001</v>
+      </c>
+      <c r="E12" s="39">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,4,FALSE)</f>
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="F12" s="40">
+        <v>0.751</v>
+      </c>
+      <c r="F12" s="39">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,5,FALSE)</f>
-        <v>0.75700000000000001</v>
-      </c>
-      <c r="G12" s="40">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="G12" s="39">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,6,FALSE)</f>
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="H12" s="40">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="H12" s="39">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,7,FALSE)</f>
-        <v>1.3109999999999999</v>
-      </c>
-      <c r="I12" s="40">
+        <v>1.2949999999999999</v>
+      </c>
+      <c r="I12" s="39">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,8,FALSE)</f>
-        <v>1.659</v>
-      </c>
-      <c r="J12" s="40">
+        <v>1.617</v>
+      </c>
+      <c r="J12" s="39">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,9,FALSE)</f>
-        <v>2.0819999999999999</v>
-      </c>
-      <c r="K12" s="40">
+        <v>2.0270000000000001</v>
+      </c>
+      <c r="K12" s="39">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,10,FALSE)</f>
         <v>0.2</v>
       </c>
-      <c r="L12" s="40">
+      <c r="L12" s="39">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,11,FALSE)</f>
-        <v>-0.48699999999999999</v>
-      </c>
-      <c r="M12" s="40">
+        <v>-0.45900000000000002</v>
+      </c>
+      <c r="M12" s="39">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,12,FALSE)</f>
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="N12" s="40">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="N12" s="39">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,13,FALSE)</f>
-        <v>11.352</v>
-      </c>
-      <c r="O12" s="41">
+        <v>10.784000000000001</v>
+      </c>
+      <c r="O12" s="40">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,14,FALSE)</f>
-        <v>3.2690000000000001</v>
+        <v>3.1070000000000002</v>
       </c>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="43">
         <f>C12-C11</f>
-        <v>-4.1999999999999982E-2</v>
-      </c>
-      <c r="D13" s="44">
+        <v>3.2999999999999974E-2</v>
+      </c>
+      <c r="D13" s="43">
         <f t="shared" ref="D13:O13" si="2">D12-D11</f>
-        <v>3.7000000000000144E-2</v>
-      </c>
-      <c r="E13" s="44">
+        <v>-5.5999999999999828E-2</v>
+      </c>
+      <c r="E13" s="43">
         <f t="shared" si="2"/>
-        <v>2.4000000000000021E-2</v>
-      </c>
-      <c r="F13" s="44">
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="F13" s="43">
         <f t="shared" si="2"/>
-        <v>2.5000000000000022E-2</v>
-      </c>
-      <c r="G13" s="44">
+        <v>4.9000000000000044E-2</v>
+      </c>
+      <c r="G13" s="43">
         <f t="shared" si="2"/>
-        <v>3.0000000000000027E-2</v>
-      </c>
-      <c r="H13" s="44">
+        <v>4.1000000000000036E-2</v>
+      </c>
+      <c r="H13" s="43">
         <f t="shared" si="2"/>
-        <v>4.0999999999999925E-2</v>
-      </c>
-      <c r="I13" s="44">
+        <v>2.4999999999999911E-2</v>
+      </c>
+      <c r="I13" s="43">
         <f t="shared" si="2"/>
-        <v>5.0999999999999934E-2</v>
-      </c>
-      <c r="J13" s="44">
+        <v>8.999999999999897E-3</v>
+      </c>
+      <c r="J13" s="43">
         <f t="shared" si="2"/>
-        <v>9.9999999999997868E-3</v>
-      </c>
-      <c r="K13" s="44">
+        <v>-4.4999999999999929E-2</v>
+      </c>
+      <c r="K13" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L13" s="44">
+      <c r="L13" s="43">
         <f t="shared" si="2"/>
-        <v>-8.3999999999999964E-2</v>
-      </c>
-      <c r="M13" s="44">
+        <v>-5.5999999999999994E-2</v>
+      </c>
+      <c r="M13" s="43">
         <f t="shared" si="2"/>
-        <v>3.0999999999999986E-2</v>
-      </c>
-      <c r="N13" s="44">
+        <v>1.6E-2</v>
+      </c>
+      <c r="N13" s="43">
         <f t="shared" si="2"/>
-        <v>1.7089999999999996</v>
-      </c>
-      <c r="O13" s="45">
+        <v>1.141</v>
+      </c>
+      <c r="O13" s="44">
         <f t="shared" si="2"/>
-        <v>0.19100000000000028</v>
+        <v>2.9000000000000359E-2</v>
       </c>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="46">
-        <v>1884</v>
+      <c r="C16" s="45">
+        <v>1925</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="C17" t="str">
         <f>VLOOKUP($C$16,Years!$A$1:$G$153,2,FALSE)</f>
-        <v>Early Years</v>
+        <v>Rebirth</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="C21" t="str">
         <f>VLOOKUP($C$16,Years!$A$1:$G$153,6,FALSE)</f>
-        <v>Stuff becomes the most important rating again as home runs and walks become nearly non existant. Stuff can increase your K/9, but likely not even close to modern levels (would need 200+ stuff to strike out at modern K/9). Hold Runners and Stamina most important.</v>
+        <v>Flyball pitchers with good/high movement are becoming better every year. HR Rate is down but BIP is significantly up. Control still important</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -1950,182 +1950,182 @@
       </c>
       <c r="C22" t="str">
         <f>VLOOKUP($C$16,Years!$A$1:$G$153,7,FALSE)</f>
-        <v>Defense and BABIP are the most important ratings on any card. Errors and Passed Balls happen every inning. Walks are slowly becoming IBB vs UBB. SB are still critical, but success rate drops drastically. HR are (almost) all Inside the Park</v>
+        <v>Balls in Play and Baserunning are important, HR are increasingly rare. Defense even more important as errors are now double modern eras</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-      <c r="S31" s="11"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="46"/>
+      <c r="R31" s="46"/>
+      <c r="S31" s="46"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="11"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="46"/>
+      <c r="P32" s="46"/>
+      <c r="Q32" s="46"/>
+      <c r="R32" s="46"/>
+      <c r="S32" s="46"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="46"/>
+      <c r="P33" s="46"/>
+      <c r="Q33" s="46"/>
+      <c r="R33" s="46"/>
+      <c r="S33" s="46"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="11"/>
-      <c r="S34" s="11"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="46"/>
+      <c r="M34" s="46"/>
+      <c r="N34" s="46"/>
+      <c r="O34" s="46"/>
+      <c r="P34" s="46"/>
+      <c r="Q34" s="46"/>
+      <c r="R34" s="46"/>
+      <c r="S34" s="46"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="11"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="46"/>
+      <c r="N35" s="46"/>
+      <c r="O35" s="46"/>
+      <c r="P35" s="46"/>
+      <c r="Q35" s="46"/>
+      <c r="R35" s="46"/>
+      <c r="S35" s="46"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="46"/>
+      <c r="N36" s="46"/>
+      <c r="O36" s="46"/>
+      <c r="P36" s="46"/>
+      <c r="Q36" s="46"/>
+      <c r="R36" s="46"/>
+      <c r="S36" s="46"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="11"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="46"/>
+      <c r="N37" s="46"/>
+      <c r="O37" s="46"/>
+      <c r="P37" s="46"/>
+      <c r="Q37" s="46"/>
+      <c r="R37" s="46"/>
+      <c r="S37" s="46"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="11"/>
-      <c r="S38" s="11"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
+      <c r="N38" s="46"/>
+      <c r="O38" s="46"/>
+      <c r="P38" s="46"/>
+      <c r="Q38" s="46"/>
+      <c r="R38" s="46"/>
+      <c r="S38" s="46"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="d844guijbs46d0OoTm4QfnjWUiFelBt7F75bt6OY2oKMr9wDUzFe0lWQW3n8xSr0ul27oGufWluzC99WvNFcdA==" saltValue="R6FY51Zc91IuLO496pt7WA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>

</xml_diff>

<commit_message>
PT Card List with Card Sets updated through 12/10.
</commit_message>
<xml_diff>
--- a/Tournament Era Worksheet.xlsx
+++ b/Tournament Era Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\OOTPResources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OOTP Analytics\Tournament Era\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135237BD-D401-437F-932B-8F116DDFC598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EF16FE-2BA6-41CC-951E-187A422A9A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{06CCA8F3-D635-4773-A702-800788336C23}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{06CCA8F3-D635-4773-A702-800788336C23}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="4" r:id="rId1"/>
@@ -23,14 +23,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -462,10 +454,10 @@
     <t>Stuff becomes the most important rating again as home runs and walks become nearly non existant. Stuff can increase your K/9, but likely not even close to modern levels (would need 200+ stuff to strike out at modern K/9). Hold Runners and Stamina most important.</t>
   </si>
   <si>
-    <t>SP rules are for "set and forget" roster creation, as the AI will not count it as a complete roster when the tournament "fires" unless you have 4 SP and 4 RP along with 10+ position players.</t>
+    <t>Defense and BABIP are the most important ratings on any card. Errors and Passed Balls happen every inning. Walks are slowly becoming IBB vs UBB. SB are still critical, but success rate drops drastically. HR are (almost) all Inside the Park</t>
   </si>
   <si>
-    <t>Defense and BABIP are the most important ratings on any card. Errors and Passed Balls happen every inning. Walks are slowly becoming IBB vs UBB. SB are still critical, but success rate drops drastically. HR are (almost) all Inside the Park</t>
+    <t>SP rules are for "set and forget" roster creation, as the AI will not count it as a complete roster when the tournament "fires" unless you have 8 pitchers along with 10+ position players.</t>
   </si>
 </sst>
 </file>
@@ -633,7 +625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -649,17 +641,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -681,7 +672,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1035,7 +1026,7 @@
   <dimension ref="B1:AA38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,429 +1040,429 @@
   <sheetData>
     <row r="1" spans="2:27" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="R2" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="S2" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="T2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="U2" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="V2" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="W2" s="12" t="s">
+      <c r="W2" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="X2" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="Y2" s="12" t="s">
+      <c r="Y2" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="Z2" s="12" t="s">
+      <c r="Z2" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="AA2" s="13" t="s">
+      <c r="AA2" s="12" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <f>Batting!$D$14</f>
         <v>185553</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <f>Batting!$G$14</f>
         <v>42554</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <f>Batting!$H$14</f>
         <v>28589</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="14">
         <f>Batting!$I$14</f>
         <v>8486</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="14">
         <f>Batting!$J$14</f>
         <v>866</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="14">
         <f>Batting!$K$14</f>
         <v>4613</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="14">
         <f>Batting!$AL$14</f>
         <v>14562</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="14">
         <f>Batting!$W$14</f>
         <v>1549</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="14">
         <f>Batting!$P$14</f>
         <v>34306</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L3" s="14">
         <f>Batting!$M$14</f>
         <v>2959</v>
       </c>
-      <c r="M3" s="15">
+      <c r="M3" s="14">
         <f>Batting!$N$14</f>
         <v>1129</v>
       </c>
-      <c r="N3" s="15">
+      <c r="N3" s="14">
         <f>Batting!$Q$14</f>
         <v>0.25700000000000001</v>
       </c>
-      <c r="O3" s="15">
+      <c r="O3" s="14">
         <f>Batting!$R$14</f>
         <v>0.32500000000000001</v>
       </c>
-      <c r="P3" s="15">
+      <c r="P3" s="14">
         <f>Batting!$S$14</f>
         <v>0.40300000000000002</v>
       </c>
-      <c r="Q3" s="16">
+      <c r="Q3" s="15">
         <f>Batting!$AK$14</f>
         <v>0.25647074728766012</v>
       </c>
-      <c r="R3" s="17">
+      <c r="R3" s="16">
         <f>Batting!$AB$14</f>
         <v>8.7559670781893004</v>
       </c>
-      <c r="S3" s="17">
+      <c r="S3" s="16">
         <f>Batting!$AC$14</f>
         <v>5.882510288065844</v>
       </c>
-      <c r="T3" s="17">
+      <c r="T3" s="16">
         <f>Batting!$AD$14</f>
         <v>1.7460905349794238</v>
       </c>
-      <c r="U3" s="17">
+      <c r="U3" s="16">
         <f>Batting!$AE$14</f>
         <v>0.17818930041152264</v>
       </c>
-      <c r="V3" s="17">
+      <c r="V3" s="16">
         <f>Batting!$AF$14</f>
         <v>0.94917695473251029</v>
       </c>
-      <c r="W3" s="17">
+      <c r="W3" s="16">
         <f>Batting!$AG$14</f>
         <v>0.60884773662551439</v>
       </c>
-      <c r="X3" s="17">
+      <c r="X3" s="16">
         <f>Batting!$AH$14</f>
         <v>2.9962962962962965</v>
       </c>
-      <c r="Y3" s="17">
+      <c r="Y3" s="16">
         <f>Batting!$AI$14</f>
         <v>7.0588477366255145</v>
       </c>
-      <c r="Z3" s="17">
+      <c r="Z3" s="16">
         <f>Batting!$AJ$14</f>
         <v>26.282921810699587</v>
       </c>
-      <c r="AA3" s="18">
+      <c r="AA3" s="17">
         <f>Pitching!$AI$14</f>
         <v>0.62345679012345678</v>
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <f>C16</f>
-        <v>1925</v>
-      </c>
-      <c r="C4" s="15">
+        <v>2022</v>
+      </c>
+      <c r="C4" s="14">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,4,FALSE)</f>
-        <v>136241</v>
-      </c>
-      <c r="D4" s="15">
+        <v>182052</v>
+      </c>
+      <c r="D4" s="14">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,7,FALSE)</f>
-        <v>34798</v>
-      </c>
-      <c r="E4" s="15">
+        <v>39675</v>
+      </c>
+      <c r="E4" s="14">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,8,FALSE)</f>
-        <v>25558</v>
-      </c>
-      <c r="F4" s="15">
+        <v>25877</v>
+      </c>
+      <c r="F4" s="14">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,9,FALSE)</f>
-        <v>5823</v>
-      </c>
-      <c r="G4" s="15">
+        <v>7940</v>
+      </c>
+      <c r="G4" s="14">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,10,FALSE)</f>
-        <v>1681</v>
-      </c>
-      <c r="H4" s="15">
+        <v>643</v>
+      </c>
+      <c r="H4" s="14">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,11,FALSE)</f>
-        <v>1736</v>
-      </c>
-      <c r="I4" s="15">
+        <v>5215</v>
+      </c>
+      <c r="I4" s="14">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,38,FALSE)</f>
-        <v>10944</v>
-      </c>
-      <c r="J4" s="15">
+        <v>14378</v>
+      </c>
+      <c r="J4" s="14">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,23,FALSE)</f>
-        <v>495</v>
-      </c>
-      <c r="K4" s="15">
+        <v>2046</v>
+      </c>
+      <c r="K4" s="14">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,16,FALSE)</f>
-        <v>6665</v>
-      </c>
-      <c r="L4" s="15">
+        <v>40812</v>
+      </c>
+      <c r="L4" s="14">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,13,FALSE)</f>
-        <v>2370</v>
-      </c>
-      <c r="M4" s="15">
+        <v>2486</v>
+      </c>
+      <c r="M4" s="14">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,14,FALSE)</f>
-        <v>1103</v>
-      </c>
-      <c r="N4" s="16">
+        <v>811</v>
+      </c>
+      <c r="N4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,17,FALSE)</f>
-        <v>0.28799999999999998</v>
-      </c>
-      <c r="O4" s="16">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="O4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,18,FALSE)</f>
-        <v>0.35</v>
-      </c>
-      <c r="P4" s="16">
+        <v>0.312</v>
+      </c>
+      <c r="P4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,19,FALSE)</f>
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="Q4" s="16">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="Q4" s="15">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,37,FALSE)</f>
-        <v>0.25862015018773465</v>
-      </c>
-      <c r="R4" s="17">
+        <v>0.25107651057566904</v>
+      </c>
+      <c r="R4" s="16">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,28,FALSE)</f>
-        <v>9.9366076527698457</v>
-      </c>
-      <c r="S4" s="17">
+        <v>8.1635802469135808</v>
+      </c>
+      <c r="S4" s="16">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,29,FALSE)</f>
-        <v>7.2981153626499147</v>
-      </c>
-      <c r="T4" s="17">
+        <v>5.3244855967078193</v>
+      </c>
+      <c r="T4" s="16">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,30,FALSE)</f>
-        <v>1.6627641347801256</v>
-      </c>
-      <c r="U4" s="17">
+        <v>1.6337448559670782</v>
+      </c>
+      <c r="U4" s="16">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,31,FALSE)</f>
-        <v>0.480011422044546</v>
-      </c>
-      <c r="V4" s="17">
+        <v>0.1323045267489712</v>
+      </c>
+      <c r="V4" s="16">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,32,FALSE)</f>
-        <v>0.49571673329525984</v>
-      </c>
-      <c r="W4" s="17">
+        <v>1.073045267489712</v>
+      </c>
+      <c r="W4" s="16">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,33,FALSE)</f>
-        <v>0.67675613934894341</v>
-      </c>
-      <c r="X4" s="17">
+        <v>0.51152263374485596</v>
+      </c>
+      <c r="X4" s="16">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,34,FALSE)</f>
-        <v>3.1250713877784122</v>
-      </c>
-      <c r="Y4" s="17">
+        <v>2.9584362139917695</v>
+      </c>
+      <c r="Y4" s="16">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,35,FALSE)</f>
-        <v>1.9031981724728726</v>
-      </c>
-      <c r="Z4" s="17">
+        <v>8.397530864197531</v>
+      </c>
+      <c r="Z4" s="16">
         <f>VLOOKUP($B$4,Batting!$A$1:$AL$153,36,FALSE)</f>
-        <v>32.098229583095375</v>
-      </c>
-      <c r="AA4" s="18">
+        <v>24.41604938271605</v>
+      </c>
+      <c r="AA4" s="17">
         <f>VLOOKUP($B$4,Pitching!$A$1:$AL$153,35,FALSE)</f>
-        <v>1.0937188434695913</v>
+        <v>0.52942386831275723</v>
       </c>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20">
         <f>N4-N3</f>
-        <v>3.0999999999999972E-2</v>
-      </c>
-      <c r="O5" s="21">
+        <v>-1.4000000000000012E-2</v>
+      </c>
+      <c r="O5" s="20">
         <f t="shared" ref="O5:AA5" si="0">O4-O3</f>
-        <v>2.4999999999999967E-2</v>
-      </c>
-      <c r="P5" s="21">
+        <v>-1.3000000000000012E-2</v>
+      </c>
+      <c r="P5" s="20">
         <f t="shared" si="0"/>
-        <v>3.999999999999948E-3</v>
-      </c>
-      <c r="Q5" s="22">
+        <v>-8.0000000000000071E-3</v>
+      </c>
+      <c r="Q5" s="21">
         <f t="shared" si="0"/>
-        <v>2.1494029000745374E-3</v>
-      </c>
-      <c r="R5" s="23">
+        <v>-5.3942367119910739E-3</v>
+      </c>
+      <c r="R5" s="22">
         <f t="shared" si="0"/>
-        <v>1.1806405745805453</v>
-      </c>
-      <c r="S5" s="23">
+        <v>-0.59238683127571967</v>
+      </c>
+      <c r="S5" s="22">
         <f t="shared" si="0"/>
-        <v>1.4156050745840707</v>
-      </c>
-      <c r="T5" s="23">
+        <v>-0.55802469135802468</v>
+      </c>
+      <c r="T5" s="22">
         <f t="shared" si="0"/>
-        <v>-8.3326400199298156E-2</v>
-      </c>
-      <c r="U5" s="23">
+        <v>-0.1123456790123456</v>
+      </c>
+      <c r="U5" s="22">
         <f t="shared" si="0"/>
-        <v>0.30182212163302335</v>
-      </c>
-      <c r="V5" s="23">
+        <v>-4.5884773662551448E-2</v>
+      </c>
+      <c r="V5" s="22">
         <f t="shared" si="0"/>
-        <v>-0.45346022143725045</v>
-      </c>
-      <c r="W5" s="23">
+        <v>0.12386831275720167</v>
+      </c>
+      <c r="W5" s="22">
         <f t="shared" si="0"/>
-        <v>6.7908402723429018E-2</v>
-      </c>
-      <c r="X5" s="23">
+        <v>-9.7325102880658432E-2</v>
+      </c>
+      <c r="X5" s="22">
         <f t="shared" si="0"/>
-        <v>0.12877509148211574</v>
-      </c>
-      <c r="Y5" s="23">
+        <v>-3.7860082304526976E-2</v>
+      </c>
+      <c r="Y5" s="22">
         <f t="shared" si="0"/>
-        <v>-5.1556495641526414</v>
-      </c>
-      <c r="Z5" s="23">
+        <v>1.3386831275720166</v>
+      </c>
+      <c r="Z5" s="22">
         <f t="shared" si="0"/>
-        <v>5.8153077723957871</v>
-      </c>
-      <c r="AA5" s="24">
+        <v>-1.8668724279835374</v>
+      </c>
+      <c r="AA5" s="23">
         <f t="shared" si="0"/>
-        <v>0.47026205334613447</v>
+        <v>-9.4032921810699555E-2</v>
       </c>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="L6" s="26" t="s">
+      <c r="L6" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="26" t="s">
+      <c r="M6" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="N6" s="26" t="s">
+      <c r="N6" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="26" t="s">
+      <c r="O6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="26" t="s">
+      <c r="P6" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="Q6" s="26" t="s">
+      <c r="Q6" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="R6" s="26" t="s">
+      <c r="R6" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="S6" s="26" t="s">
+      <c r="S6" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="T6" s="27" t="s">
+      <c r="T6" s="26" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C7" s="7">
@@ -1542,361 +1533,361 @@
         <f>Pitching!AH14</f>
         <v>-7.548471319929817E-2</v>
       </c>
-      <c r="T7" s="29">
+      <c r="T7" s="28">
         <f>Pitching!$E$14</f>
         <v>4.38</v>
       </c>
     </row>
     <row r="8" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B8" s="30">
+      <c r="B8" s="29">
         <f>C16</f>
-        <v>1925</v>
+        <v>2022</v>
       </c>
       <c r="C8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,24,FALSE)</f>
-        <v>136187</v>
+        <v>182052</v>
       </c>
       <c r="D8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,13,FALSE)</f>
-        <v>30933</v>
+        <v>43075.1</v>
       </c>
       <c r="E8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,15,FALSE)</f>
-        <v>18345</v>
+        <v>20817</v>
       </c>
       <c r="F8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,16,FALSE)</f>
-        <v>15658</v>
+        <v>18962</v>
       </c>
       <c r="G8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,14,FALSE)</f>
-        <v>34807</v>
+        <v>39675</v>
       </c>
       <c r="H8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,17,FALSE)</f>
-        <v>1169</v>
+        <v>5215</v>
       </c>
       <c r="I8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,20,FALSE)</f>
-        <v>10380</v>
+        <v>40812</v>
       </c>
       <c r="J8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,36,FALSE)</f>
-        <v>10827</v>
+        <v>14378</v>
       </c>
       <c r="K8" s="7">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,21,FALSE)</f>
-        <v>648</v>
+        <v>2046</v>
       </c>
       <c r="L8" s="9">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,30,FALSE)</f>
-        <v>3</v>
+        <v>8.5</v>
       </c>
       <c r="M8" s="9">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,37,FALSE)</f>
-        <v>3.1501309281350016</v>
+        <v>3.0040858650735922</v>
       </c>
       <c r="N8" s="9">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,28,FALSE)</f>
-        <v>0.3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="O8" s="9">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,6,FALSE)</f>
-        <v>4.5599999999999996</v>
+        <v>3.96</v>
       </c>
       <c r="P8" s="9">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,38,FALSE)</f>
-        <v>5.337503636892639</v>
+        <v>4.3494265859811501</v>
       </c>
       <c r="Q8" s="8">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,25,FALSE)</f>
-        <v>1.4750000000000001</v>
+        <v>1.266</v>
       </c>
       <c r="R8" s="9">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,33,FALSE)</f>
-        <v>4.0400488475091327</v>
+        <v>3.9358142943370531</v>
       </c>
       <c r="S8" s="9">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,34,FALSE)</f>
-        <v>-0.51995115249086687</v>
-      </c>
-      <c r="T8" s="29">
+        <v>-2.4185705662946866E-2</v>
+      </c>
+      <c r="T8" s="28">
         <f>VLOOKUP($B$8,Pitching!$A$1:$AL$153,5,FALSE)</f>
-        <v>5.24</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="33">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="32">
         <f>L8-L7</f>
-        <v>-4.0999999999999996</v>
-      </c>
-      <c r="M9" s="33">
+        <v>1.4000000000000004</v>
+      </c>
+      <c r="M9" s="32">
         <f t="shared" ref="M9:T9" si="1">M8-M7</f>
-        <v>0.12376004233186721</v>
-      </c>
-      <c r="N9" s="33">
+        <v>-2.2285020729542193E-2</v>
+      </c>
+      <c r="N9" s="32">
         <f t="shared" si="1"/>
-        <v>-0.7</v>
-      </c>
-      <c r="O9" s="33">
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="O9" s="32">
         <f t="shared" si="1"/>
-        <v>0.48999999999999932</v>
-      </c>
-      <c r="P9" s="33">
+        <v>-0.11000000000000032</v>
+      </c>
+      <c r="P9" s="32">
         <f t="shared" si="1"/>
-        <v>0.90913453685876977</v>
-      </c>
-      <c r="Q9" s="33">
+        <v>-7.8942514052719126E-2</v>
+      </c>
+      <c r="Q9" s="32">
         <f t="shared" si="1"/>
-        <v>0.12800000000000011</v>
-      </c>
-      <c r="R9" s="33">
+        <v>-8.0999999999999961E-2</v>
+      </c>
+      <c r="R9" s="32">
         <f t="shared" si="1"/>
-        <v>4.553356070843062E-2</v>
-      </c>
-      <c r="S9" s="33">
+        <v>-5.8700992463649015E-2</v>
+      </c>
+      <c r="S9" s="32">
         <f t="shared" si="1"/>
-        <v>-0.4444664392915687</v>
-      </c>
-      <c r="T9" s="34">
+        <v>5.1299007536351304E-2</v>
+      </c>
+      <c r="T9" s="33">
         <f t="shared" si="1"/>
-        <v>0.86000000000000032</v>
+        <v>-9.9999999999999645E-2</v>
       </c>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="H10" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="36" t="s">
+      <c r="I10" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="J10" s="36" t="s">
+      <c r="J10" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="K10" s="36" t="s">
+      <c r="K10" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="L10" s="36" t="s">
+      <c r="L10" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="M10" s="36" t="s">
+      <c r="M10" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="N10" s="36" t="s">
+      <c r="N10" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="O10" s="37" t="s">
+      <c r="O10" s="36" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="38">
         <f>FGGuts!$B$14</f>
         <v>0.32100000000000001</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="38">
         <f>FGGuts!$C$14</f>
         <v>1.2509999999999999</v>
       </c>
-      <c r="E11" s="39">
+      <c r="E11" s="38">
         <f>FGGuts!$D$14</f>
         <v>0.70099999999999996</v>
       </c>
-      <c r="F11" s="39">
+      <c r="F11" s="38">
         <f>FGGuts!$E$14</f>
         <v>0.73199999999999998</v>
       </c>
-      <c r="G11" s="39">
+      <c r="G11" s="38">
         <f>FGGuts!$F$14</f>
         <v>0.89500000000000002</v>
       </c>
-      <c r="H11" s="39">
+      <c r="H11" s="38">
         <f>FGGuts!$G$14</f>
         <v>1.27</v>
       </c>
-      <c r="I11" s="39">
+      <c r="I11" s="38">
         <f>FGGuts!$H$14</f>
         <v>1.6080000000000001</v>
       </c>
-      <c r="J11" s="39">
+      <c r="J11" s="38">
         <f>FGGuts!$I$14</f>
         <v>2.0720000000000001</v>
       </c>
-      <c r="K11" s="39">
+      <c r="K11" s="38">
         <f>FGGuts!$J$14</f>
         <v>0.2</v>
       </c>
-      <c r="L11" s="39">
+      <c r="L11" s="38">
         <f>FGGuts!$K$14</f>
         <v>-0.40300000000000002</v>
       </c>
-      <c r="M11" s="39">
+      <c r="M11" s="38">
         <f>FGGuts!$L$14</f>
         <v>0.115</v>
       </c>
-      <c r="N11" s="39">
+      <c r="N11" s="38">
         <f>FGGuts!$M$14</f>
         <v>9.6430000000000007</v>
       </c>
-      <c r="O11" s="40">
+      <c r="O11" s="39">
         <f>FGGuts!$N$14</f>
         <v>3.0779999999999998</v>
       </c>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B12" s="41">
+      <c r="B12" s="40">
         <f>C16</f>
-        <v>1925</v>
-      </c>
-      <c r="C12" s="39">
+        <v>2022</v>
+      </c>
+      <c r="C12" s="38">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,2,FALSE)</f>
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="D12" s="39">
+        <v>0.31</v>
+      </c>
+      <c r="D12" s="38">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,3,FALSE)</f>
-        <v>1.1950000000000001</v>
-      </c>
-      <c r="E12" s="39">
+        <v>1.2589999999999999</v>
+      </c>
+      <c r="E12" s="38">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,4,FALSE)</f>
-        <v>0.751</v>
-      </c>
-      <c r="F12" s="39">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="F12" s="38">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,5,FALSE)</f>
-        <v>0.78100000000000003</v>
-      </c>
-      <c r="G12" s="39">
+        <v>0.72</v>
+      </c>
+      <c r="G12" s="38">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,6,FALSE)</f>
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="H12" s="39">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="H12" s="38">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,7,FALSE)</f>
-        <v>1.2949999999999999</v>
-      </c>
-      <c r="I12" s="39">
+        <v>1.2609999999999999</v>
+      </c>
+      <c r="I12" s="38">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,8,FALSE)</f>
-        <v>1.617</v>
-      </c>
-      <c r="J12" s="39">
+        <v>1.601</v>
+      </c>
+      <c r="J12" s="38">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,9,FALSE)</f>
-        <v>2.0270000000000001</v>
-      </c>
-      <c r="K12" s="39">
+        <v>2.0720000000000001</v>
+      </c>
+      <c r="K12" s="38">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,10,FALSE)</f>
         <v>0.2</v>
       </c>
-      <c r="L12" s="39">
+      <c r="L12" s="38">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,11,FALSE)</f>
-        <v>-0.45900000000000002</v>
-      </c>
-      <c r="M12" s="39">
+        <v>-0.39700000000000002</v>
+      </c>
+      <c r="M12" s="38">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,12,FALSE)</f>
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="N12" s="39">
+        <v>0.114</v>
+      </c>
+      <c r="N12" s="38">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,13,FALSE)</f>
-        <v>10.784000000000001</v>
-      </c>
-      <c r="O12" s="40">
+        <v>9.5239999999999991</v>
+      </c>
+      <c r="O12" s="39">
         <f>VLOOKUP($B$12,FGGuts!$A$1:$N$153,14,FALSE)</f>
-        <v>3.1070000000000002</v>
+        <v>3.113</v>
       </c>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="42">
         <f>C12-C11</f>
-        <v>3.2999999999999974E-2</v>
-      </c>
-      <c r="D13" s="43">
+        <v>-1.100000000000001E-2</v>
+      </c>
+      <c r="D13" s="42">
         <f t="shared" ref="D13:O13" si="2">D12-D11</f>
-        <v>-5.5999999999999828E-2</v>
-      </c>
-      <c r="E13" s="43">
+        <v>8.0000000000000071E-3</v>
+      </c>
+      <c r="E13" s="42">
         <f t="shared" si="2"/>
-        <v>5.0000000000000044E-2</v>
-      </c>
-      <c r="F13" s="43">
+        <v>-1.2000000000000011E-2</v>
+      </c>
+      <c r="F13" s="42">
         <f t="shared" si="2"/>
-        <v>4.9000000000000044E-2</v>
-      </c>
-      <c r="G13" s="43">
+        <v>-1.2000000000000011E-2</v>
+      </c>
+      <c r="G13" s="42">
         <f t="shared" si="2"/>
-        <v>4.1000000000000036E-2</v>
-      </c>
-      <c r="H13" s="43">
+        <v>-1.100000000000001E-2</v>
+      </c>
+      <c r="H13" s="42">
         <f t="shared" si="2"/>
-        <v>2.4999999999999911E-2</v>
-      </c>
-      <c r="I13" s="43">
+        <v>-9.000000000000119E-3</v>
+      </c>
+      <c r="I13" s="42">
         <f t="shared" si="2"/>
-        <v>8.999999999999897E-3</v>
-      </c>
-      <c r="J13" s="43">
-        <f t="shared" si="2"/>
-        <v>-4.4999999999999929E-2</v>
-      </c>
-      <c r="K13" s="43">
+        <v>-7.0000000000001172E-3</v>
+      </c>
+      <c r="J13" s="42">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L13" s="43">
+      <c r="K13" s="42">
         <f t="shared" si="2"/>
-        <v>-5.5999999999999994E-2</v>
-      </c>
-      <c r="M13" s="43">
+        <v>0</v>
+      </c>
+      <c r="L13" s="42">
         <f t="shared" si="2"/>
-        <v>1.6E-2</v>
-      </c>
-      <c r="N13" s="43">
+        <v>6.0000000000000053E-3</v>
+      </c>
+      <c r="M13" s="42">
         <f t="shared" si="2"/>
-        <v>1.141</v>
-      </c>
-      <c r="O13" s="44">
+        <v>-1.0000000000000009E-3</v>
+      </c>
+      <c r="N13" s="42">
         <f t="shared" si="2"/>
-        <v>2.9000000000000359E-2</v>
+        <v>-0.11900000000000155</v>
+      </c>
+      <c r="O13" s="43">
+        <f t="shared" si="2"/>
+        <v>3.5000000000000142E-2</v>
       </c>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="45">
-        <v>1925</v>
+      <c r="C16" s="44">
+        <v>2022</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
@@ -1905,7 +1896,7 @@
       </c>
       <c r="C17" t="str">
         <f>VLOOKUP($C$16,Years!$A$1:$G$153,2,FALSE)</f>
-        <v>Rebirth</v>
+        <v>Modern</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
@@ -1914,7 +1905,7 @@
       </c>
       <c r="C18">
         <f>VLOOKUP($C$16,Years!$A$1:$G$153,3,FALSE)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
@@ -1923,7 +1914,7 @@
       </c>
       <c r="C19">
         <f>VLOOKUP($C$16,Years!$A$1:$G$153,4,FALSE)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
@@ -1932,7 +1923,7 @@
       </c>
       <c r="C20">
         <f>VLOOKUP($C$16,Years!$A$1:$G$153,5,FALSE)</f>
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
@@ -1941,7 +1932,7 @@
       </c>
       <c r="C21" t="str">
         <f>VLOOKUP($C$16,Years!$A$1:$G$153,6,FALSE)</f>
-        <v>Flyball pitchers with good/high movement are becoming better every year. HR Rate is down but BIP is significantly up. Control still important</v>
+        <v>Stuff and Movement are King</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -1950,185 +1941,185 @@
       </c>
       <c r="C22" t="str">
         <f>VLOOKUP($C$16,Years!$A$1:$G$153,7,FALSE)</f>
-        <v>Balls in Play and Baserunning are important, HR are increasingly rare. Defense even more important as errors are now double modern eras</v>
+        <v>Power, AvK are key. Eye helps. Fielding is not important</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="46"/>
-      <c r="P31" s="46"/>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="46"/>
-      <c r="S31" s="46"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="45"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="45"/>
+      <c r="P31" s="45"/>
+      <c r="Q31" s="45"/>
+      <c r="R31" s="45"/>
+      <c r="S31" s="45"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="46"/>
-      <c r="N32" s="46"/>
-      <c r="O32" s="46"/>
-      <c r="P32" s="46"/>
-      <c r="Q32" s="46"/>
-      <c r="R32" s="46"/>
-      <c r="S32" s="46"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="45"/>
+      <c r="N32" s="45"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="45"/>
+      <c r="Q32" s="45"/>
+      <c r="R32" s="45"/>
+      <c r="S32" s="45"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="46" t="s">
+      <c r="B33" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="46"/>
-      <c r="P33" s="46"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="46"/>
-      <c r="S33" s="46"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="45"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="45"/>
+      <c r="O33" s="45"/>
+      <c r="P33" s="45"/>
+      <c r="Q33" s="45"/>
+      <c r="R33" s="45"/>
+      <c r="S33" s="45"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="46"/>
-      <c r="L34" s="46"/>
-      <c r="M34" s="46"/>
-      <c r="N34" s="46"/>
-      <c r="O34" s="46"/>
-      <c r="P34" s="46"/>
-      <c r="Q34" s="46"/>
-      <c r="R34" s="46"/>
-      <c r="S34" s="46"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="45"/>
+      <c r="M34" s="45"/>
+      <c r="N34" s="45"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="45"/>
+      <c r="R34" s="45"/>
+      <c r="S34" s="45"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="46"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="46"/>
-      <c r="J35" s="46"/>
-      <c r="K35" s="46"/>
-      <c r="L35" s="46"/>
-      <c r="M35" s="46"/>
-      <c r="N35" s="46"/>
-      <c r="O35" s="46"/>
-      <c r="P35" s="46"/>
-      <c r="Q35" s="46"/>
-      <c r="R35" s="46"/>
-      <c r="S35" s="46"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="45"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="45"/>
+      <c r="O35" s="45"/>
+      <c r="P35" s="45"/>
+      <c r="Q35" s="45"/>
+      <c r="R35" s="45"/>
+      <c r="S35" s="45"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="46"/>
-      <c r="J36" s="46"/>
-      <c r="K36" s="46"/>
-      <c r="L36" s="46"/>
-      <c r="M36" s="46"/>
-      <c r="N36" s="46"/>
-      <c r="O36" s="46"/>
-      <c r="P36" s="46"/>
-      <c r="Q36" s="46"/>
-      <c r="R36" s="46"/>
-      <c r="S36" s="46"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="45"/>
+      <c r="M36" s="45"/>
+      <c r="N36" s="45"/>
+      <c r="O36" s="45"/>
+      <c r="P36" s="45"/>
+      <c r="Q36" s="45"/>
+      <c r="R36" s="45"/>
+      <c r="S36" s="45"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B37" s="46" t="s">
+      <c r="B37" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="46"/>
-      <c r="K37" s="46"/>
-      <c r="L37" s="46"/>
-      <c r="M37" s="46"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="46"/>
-      <c r="P37" s="46"/>
-      <c r="Q37" s="46"/>
-      <c r="R37" s="46"/>
-      <c r="S37" s="46"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
+      <c r="M37" s="45"/>
+      <c r="N37" s="45"/>
+      <c r="O37" s="45"/>
+      <c r="P37" s="45"/>
+      <c r="Q37" s="45"/>
+      <c r="R37" s="45"/>
+      <c r="S37" s="45"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B38" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="46"/>
-      <c r="I38" s="46"/>
-      <c r="J38" s="46"/>
-      <c r="K38" s="46"/>
-      <c r="L38" s="46"/>
-      <c r="M38" s="46"/>
-      <c r="N38" s="46"/>
-      <c r="O38" s="46"/>
-      <c r="P38" s="46"/>
-      <c r="Q38" s="46"/>
-      <c r="R38" s="46"/>
-      <c r="S38" s="46"/>
+      <c r="B38" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="45"/>
+      <c r="M38" s="45"/>
+      <c r="N38" s="45"/>
+      <c r="O38" s="45"/>
+      <c r="P38" s="45"/>
+      <c r="Q38" s="45"/>
+      <c r="R38" s="45"/>
+      <c r="S38" s="45"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="d844guijbs46d0OoTm4QfnjWUiFelBt7F75bt6OY2oKMr9wDUzFe0lWQW3n8xSr0ul27oGufWluzC99WvNFcdA==" saltValue="R6FY51Zc91IuLO496pt7WA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="A1WXoJ6um+U3S0+m0Hl5CCIt5gJ7qogQ2LtFKvhJ14mGvrLv/6YETy/7lhmlK38m0CS3IqJ5dSl+OzijpZk9Zw==" saltValue="aqyMa8HKlpnfvYchYZm/pA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
     <mergeCell ref="B38:S38"/>
     <mergeCell ref="B31:S31"/>
@@ -47014,8 +47005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373F186B-0DC0-4501-B8AD-720CFE591F98}">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J136" sqref="J136"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64:D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47057,10 +47048,10 @@
       <c r="C2">
         <v>5</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2">
         <v>7</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2">
         <v>14</v>
       </c>
       <c r="F2" t="s">
@@ -47080,10 +47071,10 @@
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3">
         <v>7</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3">
         <v>14</v>
       </c>
       <c r="F3" t="s">
@@ -47103,10 +47094,10 @@
       <c r="C4">
         <v>5</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4">
         <v>7</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4">
         <v>14</v>
       </c>
       <c r="F4" t="s">
@@ -47126,10 +47117,10 @@
       <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5">
         <v>7</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5">
         <v>14</v>
       </c>
       <c r="F5" t="s">
@@ -47149,10 +47140,10 @@
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6">
         <v>7</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6">
         <v>14</v>
       </c>
       <c r="F6" t="s">
@@ -47172,10 +47163,10 @@
       <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7">
         <v>7</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7">
         <v>14</v>
       </c>
       <c r="F7" t="s">
@@ -47195,10 +47186,10 @@
       <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8">
         <v>7</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8">
         <v>14</v>
       </c>
       <c r="F8" t="s">
@@ -47218,10 +47209,10 @@
       <c r="C9">
         <v>5</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9">
         <v>7</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9">
         <v>14</v>
       </c>
       <c r="F9" t="s">
@@ -47241,10 +47232,10 @@
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10">
         <v>7</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10">
         <v>14</v>
       </c>
       <c r="F10" t="s">
@@ -47264,10 +47255,10 @@
       <c r="C11">
         <v>5</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11">
         <v>7</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11">
         <v>14</v>
       </c>
       <c r="F11" t="s">
@@ -47287,10 +47278,10 @@
       <c r="C12">
         <v>5</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12">
         <v>7</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12">
         <v>14</v>
       </c>
       <c r="F12" t="s">
@@ -47310,10 +47301,10 @@
       <c r="C13">
         <v>5</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13">
         <v>7</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13">
         <v>14</v>
       </c>
       <c r="F13" t="s">
@@ -47333,10 +47324,10 @@
       <c r="C14">
         <v>5</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14">
         <v>7</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14">
         <v>14</v>
       </c>
       <c r="F14" t="s">
@@ -47356,10 +47347,10 @@
       <c r="C15">
         <v>5</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15">
         <v>7</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15">
         <v>14</v>
       </c>
       <c r="F15" t="s">
@@ -47379,10 +47370,10 @@
       <c r="C16">
         <v>5</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16">
         <v>7</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16">
         <v>14</v>
       </c>
       <c r="F16" t="s">
@@ -47402,10 +47393,10 @@
       <c r="C17">
         <v>5</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17">
         <v>7</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17">
         <v>14</v>
       </c>
       <c r="F17" t="s">
@@ -47425,10 +47416,10 @@
       <c r="C18">
         <v>5</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18">
         <v>7</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18">
         <v>14</v>
       </c>
       <c r="F18" t="s">
@@ -47448,10 +47439,10 @@
       <c r="C19">
         <v>5</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19">
         <v>7</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19">
         <v>14</v>
       </c>
       <c r="F19" t="s">
@@ -47471,10 +47462,10 @@
       <c r="C20">
         <v>5</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20">
         <v>7</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20">
         <v>14</v>
       </c>
       <c r="F20" t="s">
@@ -47494,10 +47485,10 @@
       <c r="C21">
         <v>5</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21">
         <v>7</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21">
         <v>14</v>
       </c>
       <c r="F21" t="s">
@@ -47517,10 +47508,10 @@
       <c r="C22">
         <v>5</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22">
         <v>7</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22">
         <v>14</v>
       </c>
       <c r="F22" t="s">
@@ -47540,10 +47531,10 @@
       <c r="C23">
         <v>5</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23">
         <v>7</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23">
         <v>14</v>
       </c>
       <c r="F23" t="s">
@@ -47563,10 +47554,10 @@
       <c r="C24">
         <v>5</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24">
         <v>7</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24">
         <v>14</v>
       </c>
       <c r="F24" t="s">
@@ -47586,10 +47577,10 @@
       <c r="C25">
         <v>5</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25">
         <v>7</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25">
         <v>14</v>
       </c>
       <c r="F25" t="s">
@@ -47609,10 +47600,10 @@
       <c r="C26">
         <v>5</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26">
         <v>7</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26">
         <v>14</v>
       </c>
       <c r="F26" t="s">
@@ -47632,10 +47623,10 @@
       <c r="C27">
         <v>5</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27">
         <v>7</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27">
         <v>14</v>
       </c>
       <c r="F27" t="s">
@@ -47655,10 +47646,10 @@
       <c r="C28">
         <v>5</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28">
         <v>7</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28">
         <v>14</v>
       </c>
       <c r="F28" t="s">
@@ -47678,10 +47669,10 @@
       <c r="C29">
         <v>5</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29">
         <v>7</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29">
         <v>14</v>
       </c>
       <c r="F29" t="s">
@@ -47701,10 +47692,10 @@
       <c r="C30">
         <v>5</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30">
         <v>7</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30">
         <v>14</v>
       </c>
       <c r="F30" t="s">
@@ -47724,10 +47715,10 @@
       <c r="C31">
         <v>5</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31">
         <v>7</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31">
         <v>14</v>
       </c>
       <c r="F31" t="s">
@@ -47747,10 +47738,10 @@
       <c r="C32">
         <v>5</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" t="s">
         <v>103</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32">
         <v>14</v>
       </c>
       <c r="F32" t="s">
@@ -47770,10 +47761,10 @@
       <c r="C33">
         <v>5</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" t="s">
         <v>103</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33">
         <v>14</v>
       </c>
       <c r="F33" t="s">
@@ -47793,10 +47784,10 @@
       <c r="C34">
         <v>5</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" t="s">
         <v>103</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34">
         <v>14</v>
       </c>
       <c r="F34" t="s">
@@ -47816,10 +47807,10 @@
       <c r="C35">
         <v>5</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" t="s">
         <v>103</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35">
         <v>14</v>
       </c>
       <c r="F35" t="s">
@@ -47839,10 +47830,10 @@
       <c r="C36">
         <v>5</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" t="s">
         <v>103</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36">
         <v>14</v>
       </c>
       <c r="F36" t="s">
@@ -47862,10 +47853,10 @@
       <c r="C37">
         <v>5</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" t="s">
         <v>103</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37">
         <v>14</v>
       </c>
       <c r="F37" t="s">
@@ -47885,10 +47876,10 @@
       <c r="C38">
         <v>5</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" t="s">
         <v>103</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E38">
         <v>14</v>
       </c>
       <c r="F38" t="s">
@@ -47908,10 +47899,10 @@
       <c r="C39">
         <v>5</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" t="s">
         <v>103</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E39">
         <v>14</v>
       </c>
       <c r="F39" t="s">
@@ -47931,10 +47922,10 @@
       <c r="C40">
         <v>5</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" t="s">
         <v>103</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E40">
         <v>14</v>
       </c>
       <c r="F40" t="s">
@@ -47954,10 +47945,10 @@
       <c r="C41">
         <v>5</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D41" t="s">
         <v>103</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E41">
         <v>14</v>
       </c>
       <c r="F41" t="s">
@@ -47977,10 +47968,10 @@
       <c r="C42">
         <v>5</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" t="s">
         <v>103</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42">
         <v>14</v>
       </c>
       <c r="F42" t="s">
@@ -48000,10 +47991,10 @@
       <c r="C43">
         <v>5</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" t="s">
         <v>103</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43">
         <v>14</v>
       </c>
       <c r="F43" t="s">
@@ -48023,10 +48014,10 @@
       <c r="C44">
         <v>5</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" t="s">
         <v>104</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44">
         <v>14</v>
       </c>
       <c r="F44" t="s">
@@ -48049,7 +48040,7 @@
       <c r="D45">
         <v>4</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45">
         <v>16</v>
       </c>
       <c r="F45" t="s">
@@ -48072,7 +48063,7 @@
       <c r="D46">
         <v>4</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E46">
         <v>16</v>
       </c>
       <c r="F46" t="s">
@@ -48095,7 +48086,7 @@
       <c r="D47">
         <v>4</v>
       </c>
-      <c r="E47" s="10">
+      <c r="E47">
         <v>16</v>
       </c>
       <c r="F47" t="s">
@@ -48118,7 +48109,7 @@
       <c r="D48">
         <v>4</v>
       </c>
-      <c r="E48" s="10">
+      <c r="E48">
         <v>16</v>
       </c>
       <c r="F48" t="s">
@@ -48141,7 +48132,7 @@
       <c r="D49">
         <v>4</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E49">
         <v>16</v>
       </c>
       <c r="F49" t="s">
@@ -48164,7 +48155,7 @@
       <c r="D50">
         <v>4</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E50">
         <v>16</v>
       </c>
       <c r="F50" t="s">
@@ -48187,7 +48178,7 @@
       <c r="D51">
         <v>4</v>
       </c>
-      <c r="E51" s="10">
+      <c r="E51">
         <v>16</v>
       </c>
       <c r="F51" t="s">
@@ -48210,7 +48201,7 @@
       <c r="D52">
         <v>4</v>
       </c>
-      <c r="E52" s="10">
+      <c r="E52">
         <v>16</v>
       </c>
       <c r="F52" t="s">
@@ -48233,7 +48224,7 @@
       <c r="D53">
         <v>4</v>
       </c>
-      <c r="E53" s="10">
+      <c r="E53">
         <v>16</v>
       </c>
       <c r="F53" t="s">
@@ -48256,7 +48247,7 @@
       <c r="D54">
         <v>4</v>
       </c>
-      <c r="E54" s="10">
+      <c r="E54">
         <v>16</v>
       </c>
       <c r="F54" t="s">
@@ -48279,7 +48270,7 @@
       <c r="D55">
         <v>4</v>
       </c>
-      <c r="E55" s="10">
+      <c r="E55">
         <v>16</v>
       </c>
       <c r="F55" t="s">
@@ -48302,7 +48293,7 @@
       <c r="D56">
         <v>4</v>
       </c>
-      <c r="E56" s="10">
+      <c r="E56">
         <v>16</v>
       </c>
       <c r="F56" t="s">
@@ -48325,7 +48316,7 @@
       <c r="D57">
         <v>4</v>
       </c>
-      <c r="E57" s="10">
+      <c r="E57">
         <v>16</v>
       </c>
       <c r="F57" t="s">
@@ -48348,7 +48339,7 @@
       <c r="D58">
         <v>4</v>
       </c>
-      <c r="E58" s="10">
+      <c r="E58">
         <v>16</v>
       </c>
       <c r="F58" t="s">
@@ -48371,7 +48362,7 @@
       <c r="D59">
         <v>4</v>
       </c>
-      <c r="E59" s="10">
+      <c r="E59">
         <v>16</v>
       </c>
       <c r="F59" t="s">
@@ -48394,7 +48385,7 @@
       <c r="D60">
         <v>4</v>
       </c>
-      <c r="E60" s="10">
+      <c r="E60">
         <v>16</v>
       </c>
       <c r="F60" t="s">
@@ -48417,7 +48408,7 @@
       <c r="D61">
         <v>4</v>
       </c>
-      <c r="E61" s="10">
+      <c r="E61">
         <v>16</v>
       </c>
       <c r="F61" t="s">
@@ -48440,7 +48431,7 @@
       <c r="D62">
         <v>4</v>
       </c>
-      <c r="E62" s="10">
+      <c r="E62">
         <v>16</v>
       </c>
       <c r="F62" t="s">
@@ -48463,7 +48454,7 @@
       <c r="D63">
         <v>4</v>
       </c>
-      <c r="E63" s="10">
+      <c r="E63">
         <v>16</v>
       </c>
       <c r="F63" t="s">
@@ -48481,12 +48472,12 @@
         <v>99</v>
       </c>
       <c r="C64">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D64">
-        <v>4</v>
-      </c>
-      <c r="E64" s="10">
+        <v>5</v>
+      </c>
+      <c r="E64">
         <v>18</v>
       </c>
       <c r="F64" t="s">
@@ -48504,12 +48495,12 @@
         <v>99</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D65">
-        <v>4</v>
-      </c>
-      <c r="E65" s="10">
+        <v>5</v>
+      </c>
+      <c r="E65">
         <v>18</v>
       </c>
       <c r="F65" t="s">
@@ -48527,12 +48518,12 @@
         <v>99</v>
       </c>
       <c r="C66">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D66">
-        <v>4</v>
-      </c>
-      <c r="E66" s="10">
+        <v>5</v>
+      </c>
+      <c r="E66">
         <v>18</v>
       </c>
       <c r="F66" t="s">
@@ -48550,12 +48541,12 @@
         <v>99</v>
       </c>
       <c r="C67">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D67">
-        <v>4</v>
-      </c>
-      <c r="E67" s="10">
+        <v>5</v>
+      </c>
+      <c r="E67">
         <v>18</v>
       </c>
       <c r="F67" t="s">
@@ -48573,12 +48564,12 @@
         <v>99</v>
       </c>
       <c r="C68">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D68">
-        <v>4</v>
-      </c>
-      <c r="E68" s="10">
+        <v>5</v>
+      </c>
+      <c r="E68">
         <v>18</v>
       </c>
       <c r="F68" t="s">
@@ -48596,12 +48587,12 @@
         <v>99</v>
       </c>
       <c r="C69">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D69">
-        <v>4</v>
-      </c>
-      <c r="E69" s="10">
+        <v>5</v>
+      </c>
+      <c r="E69">
         <v>18</v>
       </c>
       <c r="F69" t="s">
@@ -48619,12 +48610,12 @@
         <v>99</v>
       </c>
       <c r="C70">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D70">
-        <v>4</v>
-      </c>
-      <c r="E70" s="10">
+        <v>5</v>
+      </c>
+      <c r="E70">
         <v>18</v>
       </c>
       <c r="F70" t="s">
@@ -48642,12 +48633,12 @@
         <v>99</v>
       </c>
       <c r="C71">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D71">
-        <v>4</v>
-      </c>
-      <c r="E71" s="10">
+        <v>5</v>
+      </c>
+      <c r="E71">
         <v>18</v>
       </c>
       <c r="F71" t="s">
@@ -48665,12 +48656,12 @@
         <v>99</v>
       </c>
       <c r="C72">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D72">
-        <v>4</v>
-      </c>
-      <c r="E72" s="10">
+        <v>5</v>
+      </c>
+      <c r="E72">
         <v>18</v>
       </c>
       <c r="F72" t="s">
@@ -48688,12 +48679,12 @@
         <v>99</v>
       </c>
       <c r="C73">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D73">
-        <v>4</v>
-      </c>
-      <c r="E73" s="10">
+        <v>5</v>
+      </c>
+      <c r="E73">
         <v>18</v>
       </c>
       <c r="F73" t="s">
@@ -48711,12 +48702,12 @@
         <v>99</v>
       </c>
       <c r="C74">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D74">
-        <v>4</v>
-      </c>
-      <c r="E74" s="10">
+        <v>5</v>
+      </c>
+      <c r="E74">
         <v>18</v>
       </c>
       <c r="F74" t="s">
@@ -48734,12 +48725,12 @@
         <v>99</v>
       </c>
       <c r="C75">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D75">
-        <v>4</v>
-      </c>
-      <c r="E75" s="10">
+        <v>5</v>
+      </c>
+      <c r="E75">
         <v>18</v>
       </c>
       <c r="F75" t="s">
@@ -48757,12 +48748,12 @@
         <v>99</v>
       </c>
       <c r="C76">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D76">
-        <v>4</v>
-      </c>
-      <c r="E76" s="10">
+        <v>5</v>
+      </c>
+      <c r="E76">
         <v>18</v>
       </c>
       <c r="F76" t="s">
@@ -48780,12 +48771,12 @@
         <v>99</v>
       </c>
       <c r="C77">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D77">
-        <v>4</v>
-      </c>
-      <c r="E77" s="10">
+        <v>5</v>
+      </c>
+      <c r="E77">
         <v>18</v>
       </c>
       <c r="F77" t="s">
@@ -48803,12 +48794,12 @@
         <v>99</v>
       </c>
       <c r="C78">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D78">
-        <v>4</v>
-      </c>
-      <c r="E78" s="10">
+        <v>5</v>
+      </c>
+      <c r="E78">
         <v>18</v>
       </c>
       <c r="F78" t="s">
@@ -48826,12 +48817,12 @@
         <v>100</v>
       </c>
       <c r="C79">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D79">
-        <v>4</v>
-      </c>
-      <c r="E79" s="10">
+        <v>5</v>
+      </c>
+      <c r="E79">
         <v>18</v>
       </c>
       <c r="F79" t="s">
@@ -48849,12 +48840,12 @@
         <v>100</v>
       </c>
       <c r="C80">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D80">
-        <v>4</v>
-      </c>
-      <c r="E80" s="10">
+        <v>5</v>
+      </c>
+      <c r="E80">
         <v>18</v>
       </c>
       <c r="F80" t="s">
@@ -48872,12 +48863,12 @@
         <v>100</v>
       </c>
       <c r="C81">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D81">
-        <v>4</v>
-      </c>
-      <c r="E81" s="10">
+        <v>5</v>
+      </c>
+      <c r="E81">
         <v>18</v>
       </c>
       <c r="F81" t="s">
@@ -48895,12 +48886,12 @@
         <v>100</v>
       </c>
       <c r="C82">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D82">
-        <v>4</v>
-      </c>
-      <c r="E82" s="10">
+        <v>5</v>
+      </c>
+      <c r="E82">
         <v>18</v>
       </c>
       <c r="F82" t="s">
@@ -48918,12 +48909,12 @@
         <v>100</v>
       </c>
       <c r="C83">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D83">
-        <v>4</v>
-      </c>
-      <c r="E83" s="10">
+        <v>5</v>
+      </c>
+      <c r="E83">
         <v>18</v>
       </c>
       <c r="F83" t="s">
@@ -48941,12 +48932,12 @@
         <v>100</v>
       </c>
       <c r="C84">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D84">
-        <v>4</v>
-      </c>
-      <c r="E84" s="10">
+        <v>5</v>
+      </c>
+      <c r="E84">
         <v>18</v>
       </c>
       <c r="F84" t="s">
@@ -48964,12 +48955,12 @@
         <v>100</v>
       </c>
       <c r="C85">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D85">
-        <v>4</v>
-      </c>
-      <c r="E85" s="10">
+        <v>5</v>
+      </c>
+      <c r="E85">
         <v>18</v>
       </c>
       <c r="F85" t="s">
@@ -48987,12 +48978,12 @@
         <v>100</v>
       </c>
       <c r="C86">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D86">
-        <v>4</v>
-      </c>
-      <c r="E86" s="10">
+        <v>5</v>
+      </c>
+      <c r="E86">
         <v>18</v>
       </c>
       <c r="F86" t="s">
@@ -49010,12 +49001,12 @@
         <v>100</v>
       </c>
       <c r="C87">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D87">
-        <v>4</v>
-      </c>
-      <c r="E87" s="10">
+        <v>5</v>
+      </c>
+      <c r="E87">
         <v>18</v>
       </c>
       <c r="F87" t="s">
@@ -49033,12 +49024,12 @@
         <v>100</v>
       </c>
       <c r="C88">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D88">
-        <v>4</v>
-      </c>
-      <c r="E88" s="10">
+        <v>5</v>
+      </c>
+      <c r="E88">
         <v>18</v>
       </c>
       <c r="F88" t="s">
@@ -49056,12 +49047,12 @@
         <v>100</v>
       </c>
       <c r="C89">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D89">
-        <v>4</v>
-      </c>
-      <c r="E89" s="10">
+        <v>5</v>
+      </c>
+      <c r="E89">
         <v>18</v>
       </c>
       <c r="F89" t="s">
@@ -49079,12 +49070,12 @@
         <v>100</v>
       </c>
       <c r="C90">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D90">
-        <v>4</v>
-      </c>
-      <c r="E90" s="10">
+        <v>5</v>
+      </c>
+      <c r="E90">
         <v>18</v>
       </c>
       <c r="F90" t="s">
@@ -49102,12 +49093,12 @@
         <v>100</v>
       </c>
       <c r="C91">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D91">
-        <v>4</v>
-      </c>
-      <c r="E91" s="10">
+        <v>5</v>
+      </c>
+      <c r="E91">
         <v>18</v>
       </c>
       <c r="F91" t="s">
@@ -49125,12 +49116,12 @@
         <v>100</v>
       </c>
       <c r="C92">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D92">
-        <v>4</v>
-      </c>
-      <c r="E92" s="10">
+        <v>5</v>
+      </c>
+      <c r="E92">
         <v>18</v>
       </c>
       <c r="F92" t="s">
@@ -49148,12 +49139,12 @@
         <v>100</v>
       </c>
       <c r="C93">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D93">
-        <v>4</v>
-      </c>
-      <c r="E93" s="10">
+        <v>5</v>
+      </c>
+      <c r="E93">
         <v>18</v>
       </c>
       <c r="F93" t="s">
@@ -49171,12 +49162,12 @@
         <v>100</v>
       </c>
       <c r="C94">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D94">
-        <v>4</v>
-      </c>
-      <c r="E94" s="10">
+        <v>5</v>
+      </c>
+      <c r="E94">
         <v>18</v>
       </c>
       <c r="F94" t="s">
@@ -49194,12 +49185,12 @@
         <v>100</v>
       </c>
       <c r="C95">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D95">
-        <v>4</v>
-      </c>
-      <c r="E95" s="10">
+        <v>5</v>
+      </c>
+      <c r="E95">
         <v>18</v>
       </c>
       <c r="F95" t="s">
@@ -49217,12 +49208,12 @@
         <v>100</v>
       </c>
       <c r="C96">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D96">
-        <v>4</v>
-      </c>
-      <c r="E96" s="10">
+        <v>5</v>
+      </c>
+      <c r="E96">
         <v>18</v>
       </c>
       <c r="F96" t="s">
@@ -49240,12 +49231,12 @@
         <v>100</v>
       </c>
       <c r="C97">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D97">
-        <v>4</v>
-      </c>
-      <c r="E97" s="10">
+        <v>5</v>
+      </c>
+      <c r="E97">
         <v>18</v>
       </c>
       <c r="F97" t="s">
@@ -49263,12 +49254,12 @@
         <v>100</v>
       </c>
       <c r="C98">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D98">
-        <v>4</v>
-      </c>
-      <c r="E98" s="10">
+        <v>5</v>
+      </c>
+      <c r="E98">
         <v>18</v>
       </c>
       <c r="F98" t="s">
@@ -49286,12 +49277,12 @@
         <v>100</v>
       </c>
       <c r="C99">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D99">
-        <v>4</v>
-      </c>
-      <c r="E99" s="10">
+        <v>5</v>
+      </c>
+      <c r="E99">
         <v>18</v>
       </c>
       <c r="F99" t="s">
@@ -49309,12 +49300,12 @@
         <v>100</v>
       </c>
       <c r="C100">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D100">
-        <v>4</v>
-      </c>
-      <c r="E100" s="10">
+        <v>5</v>
+      </c>
+      <c r="E100">
         <v>18</v>
       </c>
       <c r="F100" t="s">
@@ -49332,12 +49323,12 @@
         <v>100</v>
       </c>
       <c r="C101">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D101">
-        <v>4</v>
-      </c>
-      <c r="E101" s="10">
+        <v>5</v>
+      </c>
+      <c r="E101">
         <v>18</v>
       </c>
       <c r="F101" t="s">
@@ -49355,12 +49346,12 @@
         <v>100</v>
       </c>
       <c r="C102">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D102">
-        <v>4</v>
-      </c>
-      <c r="E102" s="10">
+        <v>5</v>
+      </c>
+      <c r="E102">
         <v>18</v>
       </c>
       <c r="F102" t="s">
@@ -49378,12 +49369,12 @@
         <v>100</v>
       </c>
       <c r="C103">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D103">
-        <v>4</v>
-      </c>
-      <c r="E103" s="10">
+        <v>5</v>
+      </c>
+      <c r="E103">
         <v>18</v>
       </c>
       <c r="F103" t="s">
@@ -49401,12 +49392,12 @@
         <v>101</v>
       </c>
       <c r="C104">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D104">
-        <v>4</v>
-      </c>
-      <c r="E104" s="10">
+        <v>5</v>
+      </c>
+      <c r="E104">
         <v>18</v>
       </c>
       <c r="F104" t="s">
@@ -49424,12 +49415,12 @@
         <v>101</v>
       </c>
       <c r="C105">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D105">
-        <v>4</v>
-      </c>
-      <c r="E105" s="10">
+        <v>5</v>
+      </c>
+      <c r="E105">
         <v>18</v>
       </c>
       <c r="F105" t="s">
@@ -49447,12 +49438,12 @@
         <v>101</v>
       </c>
       <c r="C106">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D106">
-        <v>4</v>
-      </c>
-      <c r="E106" s="10">
+        <v>5</v>
+      </c>
+      <c r="E106">
         <v>18</v>
       </c>
       <c r="F106" t="s">
@@ -49470,12 +49461,12 @@
         <v>101</v>
       </c>
       <c r="C107">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D107">
-        <v>4</v>
-      </c>
-      <c r="E107" s="10">
+        <v>5</v>
+      </c>
+      <c r="E107">
         <v>18</v>
       </c>
       <c r="F107" t="s">
@@ -49493,12 +49484,12 @@
         <v>101</v>
       </c>
       <c r="C108">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D108">
-        <v>4</v>
-      </c>
-      <c r="E108" s="10">
+        <v>5</v>
+      </c>
+      <c r="E108">
         <v>18</v>
       </c>
       <c r="F108" t="s">
@@ -49516,12 +49507,12 @@
         <v>101</v>
       </c>
       <c r="C109">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D109">
-        <v>4</v>
-      </c>
-      <c r="E109" s="10">
+        <v>5</v>
+      </c>
+      <c r="E109">
         <v>18</v>
       </c>
       <c r="F109" t="s">
@@ -49539,12 +49530,12 @@
         <v>101</v>
       </c>
       <c r="C110">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D110">
-        <v>4</v>
-      </c>
-      <c r="E110" s="10">
+        <v>5</v>
+      </c>
+      <c r="E110">
         <v>18</v>
       </c>
       <c r="F110" t="s">
@@ -49562,12 +49553,12 @@
         <v>101</v>
       </c>
       <c r="C111">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D111">
-        <v>4</v>
-      </c>
-      <c r="E111" s="10">
+        <v>5</v>
+      </c>
+      <c r="E111">
         <v>18</v>
       </c>
       <c r="F111" t="s">
@@ -49585,12 +49576,12 @@
         <v>101</v>
       </c>
       <c r="C112">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D112">
-        <v>4</v>
-      </c>
-      <c r="E112" s="10">
+        <v>5</v>
+      </c>
+      <c r="E112">
         <v>18</v>
       </c>
       <c r="F112" t="s">
@@ -49608,12 +49599,12 @@
         <v>101</v>
       </c>
       <c r="C113">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D113">
-        <v>4</v>
-      </c>
-      <c r="E113" s="10">
+        <v>5</v>
+      </c>
+      <c r="E113">
         <v>18</v>
       </c>
       <c r="F113" t="s">
@@ -49631,12 +49622,12 @@
         <v>101</v>
       </c>
       <c r="C114">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D114">
-        <v>4</v>
-      </c>
-      <c r="E114" s="10">
+        <v>5</v>
+      </c>
+      <c r="E114">
         <v>18</v>
       </c>
       <c r="F114" t="s">
@@ -49654,12 +49645,12 @@
         <v>101</v>
       </c>
       <c r="C115">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D115">
-        <v>4</v>
-      </c>
-      <c r="E115" s="10">
+        <v>5</v>
+      </c>
+      <c r="E115">
         <v>18</v>
       </c>
       <c r="F115" t="s">
@@ -49677,12 +49668,12 @@
         <v>101</v>
       </c>
       <c r="C116">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D116">
-        <v>4</v>
-      </c>
-      <c r="E116" s="10">
+        <v>5</v>
+      </c>
+      <c r="E116">
         <v>18</v>
       </c>
       <c r="F116" t="s">
@@ -49700,12 +49691,12 @@
         <v>101</v>
       </c>
       <c r="C117">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D117">
-        <v>4</v>
-      </c>
-      <c r="E117" s="10">
+        <v>5</v>
+      </c>
+      <c r="E117">
         <v>18</v>
       </c>
       <c r="F117" t="s">
@@ -49723,12 +49714,12 @@
         <v>101</v>
       </c>
       <c r="C118">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D118">
-        <v>4</v>
-      </c>
-      <c r="E118" s="10">
+        <v>5</v>
+      </c>
+      <c r="E118">
         <v>18</v>
       </c>
       <c r="F118" t="s">
@@ -49746,12 +49737,12 @@
         <v>101</v>
       </c>
       <c r="C119">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D119">
-        <v>4</v>
-      </c>
-      <c r="E119" s="10">
+        <v>5</v>
+      </c>
+      <c r="E119">
         <v>18</v>
       </c>
       <c r="F119" t="s">
@@ -49769,12 +49760,12 @@
         <v>101</v>
       </c>
       <c r="C120">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D120">
-        <v>4</v>
-      </c>
-      <c r="E120" s="10">
+        <v>5</v>
+      </c>
+      <c r="E120">
         <v>18</v>
       </c>
       <c r="F120" t="s">
@@ -49792,12 +49783,12 @@
         <v>101</v>
       </c>
       <c r="C121">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D121">
-        <v>4</v>
-      </c>
-      <c r="E121" s="10">
+        <v>5</v>
+      </c>
+      <c r="E121">
         <v>18</v>
       </c>
       <c r="F121" t="s">
@@ -49815,12 +49806,12 @@
         <v>101</v>
       </c>
       <c r="C122">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D122">
-        <v>4</v>
-      </c>
-      <c r="E122" s="10">
+        <v>5</v>
+      </c>
+      <c r="E122">
         <v>18</v>
       </c>
       <c r="F122" t="s">
@@ -49838,12 +49829,12 @@
         <v>101</v>
       </c>
       <c r="C123">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D123">
-        <v>4</v>
-      </c>
-      <c r="E123" s="10">
+        <v>5</v>
+      </c>
+      <c r="E123">
         <v>18</v>
       </c>
       <c r="F123" t="s">
@@ -49861,12 +49852,12 @@
         <v>102</v>
       </c>
       <c r="C124">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D124">
-        <v>4</v>
-      </c>
-      <c r="E124" s="10">
+        <v>5</v>
+      </c>
+      <c r="E124">
         <v>18</v>
       </c>
       <c r="F124" t="s">
@@ -49884,12 +49875,12 @@
         <v>102</v>
       </c>
       <c r="C125">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D125">
-        <v>4</v>
-      </c>
-      <c r="E125" s="10">
+        <v>5</v>
+      </c>
+      <c r="E125">
         <v>18</v>
       </c>
       <c r="F125" t="s">
@@ -49907,12 +49898,12 @@
         <v>102</v>
       </c>
       <c r="C126">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D126">
-        <v>4</v>
-      </c>
-      <c r="E126" s="10">
+        <v>5</v>
+      </c>
+      <c r="E126">
         <v>18</v>
       </c>
       <c r="F126" t="s">
@@ -49930,12 +49921,12 @@
         <v>102</v>
       </c>
       <c r="C127">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D127">
-        <v>4</v>
-      </c>
-      <c r="E127" s="10">
+        <v>5</v>
+      </c>
+      <c r="E127">
         <v>18</v>
       </c>
       <c r="F127" t="s">
@@ -49953,12 +49944,12 @@
         <v>102</v>
       </c>
       <c r="C128">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D128">
-        <v>4</v>
-      </c>
-      <c r="E128" s="10">
+        <v>5</v>
+      </c>
+      <c r="E128">
         <v>18</v>
       </c>
       <c r="F128" t="s">
@@ -49976,12 +49967,12 @@
         <v>102</v>
       </c>
       <c r="C129">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D129">
-        <v>4</v>
-      </c>
-      <c r="E129" s="10">
+        <v>5</v>
+      </c>
+      <c r="E129">
         <v>18</v>
       </c>
       <c r="F129" t="s">
@@ -49999,12 +49990,12 @@
         <v>102</v>
       </c>
       <c r="C130">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D130">
-        <v>4</v>
-      </c>
-      <c r="E130" s="10">
+        <v>5</v>
+      </c>
+      <c r="E130">
         <v>18</v>
       </c>
       <c r="F130" t="s">
@@ -50022,12 +50013,12 @@
         <v>102</v>
       </c>
       <c r="C131">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D131">
-        <v>4</v>
-      </c>
-      <c r="E131" s="10">
+        <v>5</v>
+      </c>
+      <c r="E131">
         <v>18</v>
       </c>
       <c r="F131" t="s">
@@ -50045,12 +50036,12 @@
         <v>102</v>
       </c>
       <c r="C132">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D132">
-        <v>4</v>
-      </c>
-      <c r="E132" s="10">
+        <v>5</v>
+      </c>
+      <c r="E132">
         <v>18</v>
       </c>
       <c r="F132" t="s">
@@ -50068,12 +50059,12 @@
         <v>102</v>
       </c>
       <c r="C133">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D133">
-        <v>4</v>
-      </c>
-      <c r="E133" s="10">
+        <v>5</v>
+      </c>
+      <c r="E133">
         <v>18</v>
       </c>
       <c r="F133" t="s">
@@ -50091,12 +50082,12 @@
         <v>102</v>
       </c>
       <c r="C134">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D134">
-        <v>4</v>
-      </c>
-      <c r="E134" s="10">
+        <v>5</v>
+      </c>
+      <c r="E134">
         <v>18</v>
       </c>
       <c r="F134" t="s">
@@ -50114,12 +50105,12 @@
         <v>102</v>
       </c>
       <c r="C135">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D135">
-        <v>4</v>
-      </c>
-      <c r="E135" s="10">
+        <v>5</v>
+      </c>
+      <c r="E135">
         <v>18</v>
       </c>
       <c r="F135" t="s">
@@ -50137,12 +50128,12 @@
         <v>102</v>
       </c>
       <c r="C136">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D136">
-        <v>4</v>
-      </c>
-      <c r="E136" s="10">
+        <v>5</v>
+      </c>
+      <c r="E136">
         <v>18</v>
       </c>
       <c r="F136" t="s">
@@ -50160,12 +50151,12 @@
         <v>102</v>
       </c>
       <c r="C137">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D137">
-        <v>4</v>
-      </c>
-      <c r="E137" s="10">
+        <v>5</v>
+      </c>
+      <c r="E137">
         <v>18</v>
       </c>
       <c r="F137" t="s">
@@ -50183,12 +50174,12 @@
         <v>102</v>
       </c>
       <c r="C138">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D138">
-        <v>4</v>
-      </c>
-      <c r="E138" s="10">
+        <v>5</v>
+      </c>
+      <c r="E138">
         <v>18</v>
       </c>
       <c r="F138" t="s">
@@ -50206,12 +50197,12 @@
         <v>102</v>
       </c>
       <c r="C139">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D139">
-        <v>4</v>
-      </c>
-      <c r="E139" s="10">
+        <v>5</v>
+      </c>
+      <c r="E139">
         <v>18</v>
       </c>
       <c r="F139" t="s">
@@ -50229,19 +50220,19 @@
         <v>102</v>
       </c>
       <c r="C140">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D140">
-        <v>4</v>
-      </c>
-      <c r="E140" s="10">
+        <v>5</v>
+      </c>
+      <c r="E140">
         <v>18</v>
       </c>
       <c r="F140" t="s">
         <v>140</v>
       </c>
       <c r="G140" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -50252,19 +50243,19 @@
         <v>102</v>
       </c>
       <c r="C141">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D141">
-        <v>4</v>
-      </c>
-      <c r="E141" s="10">
+        <v>5</v>
+      </c>
+      <c r="E141">
         <v>18</v>
       </c>
       <c r="F141" t="s">
         <v>140</v>
       </c>
       <c r="G141" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -50275,19 +50266,19 @@
         <v>102</v>
       </c>
       <c r="C142">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D142">
-        <v>4</v>
-      </c>
-      <c r="E142" s="10">
+        <v>5</v>
+      </c>
+      <c r="E142">
         <v>18</v>
       </c>
       <c r="F142" t="s">
         <v>140</v>
       </c>
       <c r="G142" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -50298,19 +50289,19 @@
         <v>102</v>
       </c>
       <c r="C143">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D143">
-        <v>4</v>
-      </c>
-      <c r="E143" s="10">
+        <v>5</v>
+      </c>
+      <c r="E143">
         <v>18</v>
       </c>
       <c r="F143" t="s">
         <v>140</v>
       </c>
       <c r="G143" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -50321,19 +50312,19 @@
         <v>102</v>
       </c>
       <c r="C144">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D144">
-        <v>4</v>
-      </c>
-      <c r="E144" s="10">
+        <v>5</v>
+      </c>
+      <c r="E144">
         <v>18</v>
       </c>
       <c r="F144" t="s">
         <v>140</v>
       </c>
       <c r="G144" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -50344,19 +50335,19 @@
         <v>102</v>
       </c>
       <c r="C145">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D145">
-        <v>4</v>
-      </c>
-      <c r="E145" s="10">
+        <v>5</v>
+      </c>
+      <c r="E145">
         <v>18</v>
       </c>
       <c r="F145" t="s">
         <v>140</v>
       </c>
       <c r="G145" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -50367,19 +50358,19 @@
         <v>102</v>
       </c>
       <c r="C146">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D146">
-        <v>4</v>
-      </c>
-      <c r="E146" s="10">
+        <v>5</v>
+      </c>
+      <c r="E146">
         <v>18</v>
       </c>
       <c r="F146" t="s">
         <v>140</v>
       </c>
       <c r="G146" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -50390,19 +50381,19 @@
         <v>102</v>
       </c>
       <c r="C147">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D147">
-        <v>4</v>
-      </c>
-      <c r="E147" s="10">
+        <v>5</v>
+      </c>
+      <c r="E147">
         <v>18</v>
       </c>
       <c r="F147" t="s">
         <v>140</v>
       </c>
       <c r="G147" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -50413,19 +50404,19 @@
         <v>102</v>
       </c>
       <c r="C148">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D148">
-        <v>4</v>
-      </c>
-      <c r="E148" s="10">
+        <v>5</v>
+      </c>
+      <c r="E148">
         <v>18</v>
       </c>
       <c r="F148" t="s">
         <v>140</v>
       </c>
       <c r="G148" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -50436,19 +50427,19 @@
         <v>102</v>
       </c>
       <c r="C149">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D149">
-        <v>4</v>
-      </c>
-      <c r="E149" s="10">
+        <v>5</v>
+      </c>
+      <c r="E149">
         <v>18</v>
       </c>
       <c r="F149" t="s">
         <v>140</v>
       </c>
       <c r="G149" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -50459,19 +50450,19 @@
         <v>102</v>
       </c>
       <c r="C150">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D150">
-        <v>4</v>
-      </c>
-      <c r="E150" s="10">
+        <v>5</v>
+      </c>
+      <c r="E150">
         <v>18</v>
       </c>
       <c r="F150" t="s">
         <v>140</v>
       </c>
       <c r="G150" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -50482,19 +50473,19 @@
         <v>102</v>
       </c>
       <c r="C151">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D151">
-        <v>4</v>
-      </c>
-      <c r="E151" s="10">
+        <v>5</v>
+      </c>
+      <c r="E151">
         <v>18</v>
       </c>
       <c r="F151" t="s">
         <v>140</v>
       </c>
       <c r="G151" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -50505,19 +50496,19 @@
         <v>102</v>
       </c>
       <c r="C152">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D152">
-        <v>4</v>
-      </c>
-      <c r="E152" s="10">
+        <v>5</v>
+      </c>
+      <c r="E152">
         <v>18</v>
       </c>
       <c r="F152" t="s">
         <v>140</v>
       </c>
       <c r="G152" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -50528,19 +50519,19 @@
         <v>102</v>
       </c>
       <c r="C153">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D153">
-        <v>4</v>
-      </c>
-      <c r="E153" s="10">
+        <v>5</v>
+      </c>
+      <c r="E153">
         <v>18</v>
       </c>
       <c r="F153" t="s">
         <v>140</v>
       </c>
       <c r="G153" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>